<commit_message>
First set of training data
began creating training data, not certain if this will work as intended. Also wrote python script to reformat cube explorer scrambles into the format our solver uses.
</commit_message>
<xml_diff>
--- a/Parts spreadsheet.xlsx
+++ b/Parts spreadsheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17925" windowHeight="8730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,10 +67,18 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,14 +101,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,7 +393,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +432,7 @@
         <f>C2*B2</f>
         <v>159.80000000000001</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -430,16 +441,16 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
         <v>7.99</v>
       </c>
       <c r="D3" s="1">
         <f>C3*B3</f>
-        <v>23.97</v>
-      </c>
-      <c r="E3" t="s">
+        <v>15.98</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -457,7 +468,7 @@
         <f t="shared" ref="D4:D5" si="0">C4*B4</f>
         <v>89.699999999999989</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -475,17 +486,23 @@
         <f t="shared" si="0"/>
         <v>89.699999999999989</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D7" s="1">
         <f>SUM(D2:D5)</f>
-        <v>363.17</v>
+        <v>355.18</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{E950B4B7-51CD-44E0-A0D0-4D7D29910A21}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{56211C76-3679-4E9C-828F-1C126A0E4698}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{B5BEF17A-6C58-45AF-85E1-5A9315954897}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{7CF73344-EE84-4F2C-BDD4-BEF4DEFE0C63}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>